<commit_message>
[ANV] updating decay chain spreadsheet
</commit_message>
<xml_diff>
--- a/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/2-Flux/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E261B43F-3B59-9B43-B643-4CAA6E2C2A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DFC1DC-F823-384E-94EC-D1219988B456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -17,10 +17,10 @@
     <sheet name="U235" sheetId="2" r:id="rId2"/>
     <sheet name="U238" sheetId="3" r:id="rId3"/>
     <sheet name="SE Results" sheetId="4" r:id="rId4"/>
-    <sheet name="1ppb" sheetId="6" r:id="rId5"/>
+    <sheet name="SE (1ppb)" sheetId="6" r:id="rId5"/>
     <sheet name="Shotcrete Density" sheetId="5" r:id="rId6"/>
     <sheet name="Shotcrete Hang" sheetId="7" r:id="rId7"/>
-    <sheet name="Target Fractions" sheetId="8" r:id="rId8"/>
+    <sheet name="Shotcrete Target Fractions" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -308,7 +308,7 @@
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -415,9 +415,9 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,7 +1605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA6BC9F-6F57-874B-973E-14E935690D92}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2164,7 +2164,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2889,7 +2889,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4469,15 +4469,15 @@
         <v>0.04</v>
       </c>
       <c r="F6" s="25">
-        <f t="shared" ref="F5:F36" si="0">B6*(D6+E6)/200</f>
+        <f t="shared" ref="F6:F36" si="0">B6*(D6+E6)/200</f>
         <v>2.4262682539746976E-4</v>
       </c>
       <c r="G6" s="25">
-        <f t="shared" ref="G5:G36" si="1">B6*D6/100</f>
+        <f t="shared" ref="G6:G36" si="1">B6*D6/100</f>
         <v>2.3218786159288506E-4</v>
       </c>
       <c r="H6" s="25">
-        <f t="shared" ref="H5:H36" si="2">B6*E6/100</f>
+        <f t="shared" ref="H6:H36" si="2">B6*E6/100</f>
         <v>2.5306578920205453E-4</v>
       </c>
       <c r="I6" s="25">

</xml_diff>

<commit_message>
[ANV] updated decay chains spreadsheet
</commit_message>
<xml_diff>
--- a/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/2-Flux/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0CECBB-FEDC-E949-975E-F02CF4886AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C06051-3EAE-BF49-A260-AD25E699BC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" firstSheet="3" activeTab="10" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" firstSheet="5" activeTab="13" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="HDPE Target Fractions" sheetId="10" r:id="rId10"/>
     <sheet name="Cu Density" sheetId="12" r:id="rId11"/>
     <sheet name="Cu Target Fractions " sheetId="11" r:id="rId12"/>
+    <sheet name="Pb Density" sheetId="13" r:id="rId13"/>
+    <sheet name="Pb Target Fractions" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="91">
   <si>
     <t>Decay</t>
   </si>
@@ -314,6 +316,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Copper</t>
+  </si>
+  <si>
+    <t>Pb</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Lead</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1107,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1E71AD-7B86-084C-935A-71150EDA902D}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1456,6 +1464,323 @@
       <c r="C5" s="23"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB9F476-C16E-F542-A930-1F8245D1666E}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>82</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>11340</v>
+      </c>
+      <c r="E2">
+        <f>D2*(1000)*(1/100000)</f>
+        <v>113.4</v>
+      </c>
+      <c r="F2">
+        <f>$E$2*(C2/100)</f>
+        <v>1.1340000000000001</v>
+      </c>
+      <c r="G2">
+        <v>207.2</v>
+      </c>
+      <c r="H2">
+        <f>(F2/G2)*6.0221408E+23</f>
+        <v>3.2959013837837839E+21</v>
+      </c>
+      <c r="I2">
+        <f>H2/$H$3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="7">
+        <f>SUM(C2:C2)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <f>SUM(F2:F2)</f>
+        <v>1.1340000000000001</v>
+      </c>
+      <c r="H3" s="7">
+        <f>SUM(H2:H2)</f>
+        <v>3.2959013837837839E+21</v>
+      </c>
+      <c r="I3" s="7">
+        <f>SUM(I2:I2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB323B4-ACF2-0B48-8FDD-57E99702E4D7}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="22" customWidth="1"/>
+    <col min="4" max="4" width="22" style="25" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="22">
+        <v>204</v>
+      </c>
+      <c r="D3" s="25">
+        <f>1.4*(1-0.06)</f>
+        <v>1.3159999999999998</v>
+      </c>
+      <c r="E3" s="25">
+        <f>1.4*(1+0.06)</f>
+        <v>1.484</v>
+      </c>
+      <c r="F3" s="25">
+        <f t="shared" ref="F3:F6" si="0">B3*(D3+E3)/200</f>
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="G3" s="25">
+        <f t="shared" ref="G3:G6" si="1">B3*D3/100</f>
+        <v>1.3159999999999998E-2</v>
+      </c>
+      <c r="H3" s="25">
+        <f t="shared" ref="H3:H6" si="2">B3*E3/100</f>
+        <v>1.4839999999999999E-2</v>
+      </c>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="22">
+        <v>206</v>
+      </c>
+      <c r="D4" s="25">
+        <f>24.1*(0.7)</f>
+        <v>16.87</v>
+      </c>
+      <c r="E4" s="25">
+        <f>24.1*1.3</f>
+        <v>31.330000000000002</v>
+      </c>
+      <c r="F4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.24100000000000002</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="1"/>
+        <v>0.16870000000000002</v>
+      </c>
+      <c r="H4" s="25">
+        <f t="shared" si="2"/>
+        <v>0.31330000000000002</v>
+      </c>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <v>207</v>
+      </c>
+      <c r="D5" s="25">
+        <f>22.1*0.5</f>
+        <v>11.05</v>
+      </c>
+      <c r="E5" s="25">
+        <f>22.1*1.5</f>
+        <v>33.150000000000006</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.221</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="1"/>
+        <v>0.1105</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="2"/>
+        <v>0.33150000000000007</v>
+      </c>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="22">
+        <v>208</v>
+      </c>
+      <c r="D6" s="25">
+        <f>52.4-0.7</f>
+        <v>51.699999999999996</v>
+      </c>
+      <c r="E6" s="25">
+        <f>52.4+0.7</f>
+        <v>53.1</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" si="0"/>
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5169999999999999</v>
+      </c>
+      <c r="H6" s="25">
+        <f t="shared" si="2"/>
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="16">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4737,7 +5062,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5644,7 +5969,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[ANV] added Pb to the estimation of volumetric SOURCES
</commit_message>
<xml_diff>
--- a/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/2-Flux/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C06051-3EAE-BF49-A260-AD25E699BC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205B030F-2A48-D940-A0A9-B0620E812CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" firstSheet="5" activeTab="13" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" firstSheet="5" activeTab="12" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -1345,7 +1345,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB9F476-C16E-F542-A930-1F8245D1666E}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1603,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB323B4-ACF2-0B48-8FDD-57E99702E4D7}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[ANV] updated the SOURCES running
</commit_message>
<xml_diff>
--- a/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/2-Flux/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/2-Flux/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205B030F-2A48-D940-A0A9-B0620E812CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72FE57-FDD0-D344-BD2E-36AB6EC76613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" firstSheet="5" activeTab="12" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" firstSheet="2" activeTab="10" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,11 @@
     <sheet name="Shotcrete Target Fractions" sheetId="8" r:id="rId8"/>
     <sheet name="HDPE Density" sheetId="9" r:id="rId9"/>
     <sheet name="HDPE Target Fractions" sheetId="10" r:id="rId10"/>
-    <sheet name="Cu Density" sheetId="12" r:id="rId11"/>
-    <sheet name="Cu Target Fractions " sheetId="11" r:id="rId12"/>
-    <sheet name="Pb Density" sheetId="13" r:id="rId13"/>
-    <sheet name="Pb Target Fractions" sheetId="14" r:id="rId14"/>
+    <sheet name="Cu SE (1ppb)" sheetId="15" r:id="rId11"/>
+    <sheet name="Cu Density" sheetId="12" r:id="rId12"/>
+    <sheet name="Cu Target Fractions " sheetId="11" r:id="rId13"/>
+    <sheet name="Pb Density" sheetId="13" r:id="rId14"/>
+    <sheet name="Pb Target Fractions" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="91">
   <si>
     <t>Decay</t>
   </si>
@@ -1212,6 +1213,731 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD987785-DFCA-F741-AC6F-E5A525B26230}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2*($D$2/0.00000000000003)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:E8" si="0">$F$2*C2</f>
+        <v>99900000000000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>9.9899999999999993E+22</v>
+      </c>
+      <c r="G2" s="11">
+        <v>4.0815999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6">
+        <f>4.07056E-24</f>
+        <v>4.0705599999999999E-24</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C8" si="1">B3*($D$2/0.00000000000003)</f>
+        <v>1.3568533333333334E-19</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>13554.9648</v>
+      </c>
+      <c r="G3" s="11">
+        <v>5.5201500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6">
+        <f>2.11268E-26</f>
+        <v>2.1126800000000001E-26</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="1"/>
+        <v>7.0422666666666678E-22</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>70.352243999999999</v>
+      </c>
+      <c r="G4" s="11">
+        <v>5.7889214999999998</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.7546900000000003E-30</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2515633333333336E-25</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2503117700000002E-2</v>
+      </c>
+      <c r="G5" s="11">
+        <v>6.4047409999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="13">
+        <v>9.8039200000000002E-33</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="1"/>
+        <v>3.2679733333333338E-28</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>3.2647053600000002E-5</v>
+      </c>
+      <c r="G6" s="14">
+        <v>6.9063499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1.2898000000000001E-38</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="1"/>
+        <v>4.299333333333334E-34</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>4.2950340000000007E-11</v>
+      </c>
+      <c r="G7" s="14">
+        <v>8.9541910999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13">
+        <f>2.45902E-28</f>
+        <v>2.4590199999999999E-28</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="1"/>
+        <v>8.1967333333333338E-24</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.81885366000000004</v>
+      </c>
+      <c r="G8" s="14">
+        <v>6.2072630000000002</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8.9999999999999995E-15</v>
+      </c>
+      <c r="C11" s="6">
+        <f>B11*($D$11/0.000000000000009)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E11" s="6">
+        <f>$F$11*C11</f>
+        <v>99900000000000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>9.9899999999999993E+22</v>
+      </c>
+      <c r="G11" s="11">
+        <v>4.2699210000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6">
+        <f>4.94533E-19</f>
+        <v>4.9453300000000002E-19</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:C22" si="2">B12*($D$11/0.000000000000009)</f>
+        <v>5.4948111111111116E-14</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:E22" si="3">$F$11*C12</f>
+        <v>5489316300</v>
+      </c>
+      <c r="G12" s="11">
+        <v>4.8575699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6">
+        <f>1.51782E-19</f>
+        <v>1.5178200000000001E-19</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6864666666666669E-14</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="3"/>
+        <v>1684780200.0000002</v>
+      </c>
+      <c r="G13" s="11">
+        <v>4.7700149999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6">
+        <f>3.22604E-21</f>
+        <v>3.22604E-21</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5844888888888891E-16</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="3"/>
+        <v>35809044</v>
+      </c>
+      <c r="G14" s="11">
+        <v>4.87073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2.1078800000000001E-26</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3420888888888894E-21</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="3"/>
+        <v>233.97468000000003</v>
+      </c>
+      <c r="G15" s="11">
+        <v>5.5904299999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1.9150299999999999E-35</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="2"/>
+        <v>2.1278111111111113E-30</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="13">
+        <f t="shared" si="3"/>
+        <v>2.1256833000000001E-7</v>
+      </c>
+      <c r="G16" s="14">
+        <v>6.8762999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1.1858500000000001E-29</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3176111111111114E-24</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.13162935000000001</v>
+      </c>
+      <c r="G17" s="11">
+        <v>6.1147590000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1.04395E-35</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="2"/>
+        <v>1.1599444444444446E-30</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="3"/>
+        <v>1.1587845E-7</v>
+      </c>
+      <c r="G18" s="14">
+        <v>7.8335460000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.62767E-25</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="2"/>
+        <v>8.4751888888888893E-20</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="3"/>
+        <v>8466.7137000000002</v>
+      </c>
+      <c r="G19" s="11">
+        <v>5.4075369999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="13">
+        <v>7.6275999999999997E-29</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="2"/>
+        <v>8.4751111111111123E-24</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="3"/>
+        <v>0.84666360000000007</v>
+      </c>
+      <c r="G20" s="14">
+        <v>5.6212999999999997</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.7609400000000002E-26</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0677111111111118E-21</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="3"/>
+        <v>306.46434000000005</v>
+      </c>
+      <c r="G21" s="11">
+        <v>5.0365799999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4.47794E-23</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="2"/>
+        <v>4.9754888888888893E-18</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="3"/>
+        <v>497051.34</v>
+      </c>
+      <c r="G22" s="11">
+        <v>3.7921999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.4836000000000002E-17</v>
+      </c>
+      <c r="C26" s="6">
+        <f>B26*($D$26/6.4836E-17)</f>
+        <v>7.2040000000000004E-12</v>
+      </c>
+      <c r="D26" s="8">
+        <f>0.007204*D11</f>
+        <v>7.2040000000000004E-12</v>
+      </c>
+      <c r="E26" s="6">
+        <f>$F$26*C26</f>
+        <v>719679600000</v>
+      </c>
+      <c r="F26" s="6">
+        <v>9.9899999999999993E+22</v>
+      </c>
+      <c r="G26" s="11">
+        <v>4.6781699999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.0157699999999998E-21</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" ref="C27:C37" si="4">B27*($D$26/6.4836E-17)</f>
+        <v>3.3508555555555554E-16</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" ref="E27:E37" si="5">$F$26*C27</f>
+        <v>33475046.999999996</v>
+      </c>
+      <c r="G27" s="11">
+        <v>5.1499800000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4.6674600000000001E-27</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="4"/>
+        <v>5.1860666666666665E-22</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="5"/>
+        <v>51.808805999999997</v>
+      </c>
+      <c r="G28" s="11">
+        <v>6.1466010000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2.0074E-24</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="4"/>
+        <v>2.2304444444444444E-19</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="5"/>
+        <v>22282.14</v>
+      </c>
+      <c r="G29" s="11">
+        <v>5.0422713999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2.8817300000000002E-27</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="4"/>
+        <v>3.2019222222222224E-22</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="5"/>
+        <v>31.987203000000001</v>
+      </c>
+      <c r="G30" s="11">
+        <v>5.9789921000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="6">
+        <v>5.32606E-32</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="4"/>
+        <v>5.9178444444444445E-27</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="5"/>
+        <v>5.9119266000000001E-4</v>
+      </c>
+      <c r="G31" s="11">
+        <v>5.5613000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1.15793E-32</v>
+      </c>
+      <c r="C32" s="13">
+        <f t="shared" si="4"/>
+        <v>1.2865888888888888E-27</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="5"/>
+        <v>1.2853022999999999E-4</v>
+      </c>
+      <c r="G32" s="14">
+        <v>6.9462299999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1.3557199999999999E-35</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="4"/>
+        <v>1.5063555555555554E-30</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="5"/>
+        <v>1.5048491999999996E-7</v>
+      </c>
+      <c r="G33" s="11">
+        <v>6.3425000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2.9209100000000002E-37</v>
+      </c>
+      <c r="C34" s="13">
+        <f t="shared" si="4"/>
+        <v>3.2454555555555558E-32</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="5"/>
+        <v>3.2422101000000002E-9</v>
+      </c>
+      <c r="G34" s="14">
+        <v>8.1783999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5.1875399999999997E-36</v>
+      </c>
+      <c r="C35" s="13">
+        <f t="shared" si="4"/>
+        <v>5.7639333333333326E-31</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="5"/>
+        <v>5.7581693999999988E-8</v>
+      </c>
+      <c r="G35" s="14">
+        <v>7.5263799999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1.50413E-33</v>
+      </c>
+      <c r="C36" s="13">
+        <f t="shared" si="4"/>
+        <v>1.6712555555555556E-28</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="5"/>
+        <v>1.6695842999999998E-5</v>
+      </c>
+      <c r="G36" s="14">
+        <v>7.5946499999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="13">
+        <v>3.7490899999999998E-31</v>
+      </c>
+      <c r="C37" s="13">
+        <f t="shared" si="4"/>
+        <v>4.1656555555555551E-26</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="5"/>
+        <v>4.161489899999999E-3</v>
+      </c>
+      <c r="G37" s="14">
+        <v>6.7504499999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1E71AD-7B86-084C-935A-71150EDA902D}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -1340,7 +2066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51A60A3-E749-C640-A85B-BE199B31A592}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -1470,11 +2196,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB9F476-C16E-F542-A930-1F8245D1666E}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1599,7 +2325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB323B4-ACF2-0B48-8FDD-57E99702E4D7}">
   <dimension ref="A1:I7"/>
   <sheetViews>

</xml_diff>